<commit_message>
Add excel utilities (#9)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -17,6 +17,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silva</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,8 +109,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -110,14 +135,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Add testNG reports feature
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -20,21 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">firstName</t>
+    <t xml:space="preserve">firstaame</t>
   </si>
   <si>
-    <t xml:space="preserve">lastName</t>
+    <t xml:space="preserve">lastname</t>
   </si>
   <si>
-    <t xml:space="preserve">postCode</t>
+    <t xml:space="preserve">postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alerttext</t>
   </si>
   <si>
     <t xml:space="preserve">Joao</t>
   </si>
   <si>
     <t xml:space="preserve">Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer added successfully</t>
   </si>
 </sst>
 </file>
@@ -135,13 +141,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -153,16 +159,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>123456</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add testNG reports feature (#10)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -20,21 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">firstName</t>
+    <t xml:space="preserve">firstaame</t>
   </si>
   <si>
-    <t xml:space="preserve">lastName</t>
+    <t xml:space="preserve">lastname</t>
   </si>
   <si>
-    <t xml:space="preserve">postCode</t>
+    <t xml:space="preserve">postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alerttext</t>
   </si>
   <si>
     <t xml:space="preserve">Joao</t>
   </si>
   <si>
     <t xml:space="preserve">Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer added successfully</t>
   </si>
 </sst>
 </file>
@@ -135,13 +141,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -153,16 +159,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>123456</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add parameters to tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">firstaame</t>
   </si>
@@ -44,16 +44,28 @@
     <t xml:space="preserve">Customer added successfully</t>
   </si>
   <si>
+    <t xml:space="preserve">Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alvez</t>
+  </si>
+  <si>
     <t xml:space="preserve">customer</t>
   </si>
   <si>
     <t xml:space="preserve">currency</t>
   </si>
   <si>
-    <t xml:space="preserve">Jose Silva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real</t>
+    <t xml:space="preserve">Joao Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dollar</t>
   </si>
 </sst>
 </file>
@@ -154,13 +166,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -187,6 +199,34 @@
         <v>123456</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>654321</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>123654</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -208,26 +248,26 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>8</v>
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add run mode option
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="test_suite" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t xml:space="preserve">firstaame</t>
   </si>
@@ -66,6 +67,27 @@
   </si>
   <si>
     <t xml:space="preserve">Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runmode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddCustomerTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenAccountTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
   </si>
 </sst>
 </file>
@@ -75,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -96,6 +118,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,12 +169,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,11 +201,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -203,13 +236,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>654321</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -217,13 +250,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>123654</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -252,22 +285,78 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
+      <c r="A2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add hashtable use to parameters
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,9 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">firstaame</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">firstname</t>
   </si>
   <si>
     <t xml:space="preserve">lastname</t>
@@ -36,6 +36,9 @@
     <t xml:space="preserve">alerttext</t>
   </si>
   <si>
+    <t xml:space="preserve">runmode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joao</t>
   </si>
   <si>
@@ -45,18 +48,30 @@
     <t xml:space="preserve">Customer added successfully</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maria</t>
   </si>
   <si>
     <t xml:space="preserve">Santos</t>
   </si>
   <si>
-    <t xml:space="preserve">Enzo</t>
+    <t xml:space="preserve">Jose</t>
   </si>
   <si>
     <t xml:space="preserve">Alvez</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jorge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Souza</t>
+  </si>
+  <si>
     <t xml:space="preserve">customer</t>
   </si>
   <si>
@@ -78,16 +93,10 @@
     <t xml:space="preserve">BankManagerLoginTest</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">AddCustomerTest</t>
   </si>
   <si>
     <t xml:space="preserve">OpenAccountTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
   </si>
 </sst>
 </file>
@@ -199,13 +208,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -220,47 +232,76 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>654321</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>123654</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>789456</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -279,28 +320,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -321,42 +371,42 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>